<commit_message>
Commit prior to branching for mtDNA ddPCR analysis. Includes addition of Taqman manufacturing files.
</commit_message>
<xml_diff>
--- a/resources/mosaic_targets_v2.xlsx
+++ b/resources/mosaic_targets_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Regional Genetics Service\Validation Documents\Mosaic\ddPCR\ddpcr_mosaicism\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B9BDA0-823F-42A4-85A3-491E45646FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D1451C-C5BE-4AA9-A56B-C34C31E4AA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mosaicism_targets_v2" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="168">
   <si>
     <t>assay_id</t>
   </si>
@@ -66,418 +66,502 @@
     <t>assay_name</t>
   </si>
   <si>
+    <t>channel2_target</t>
+  </si>
+  <si>
+    <t>channel1_category</t>
+  </si>
+  <si>
+    <t>channel2_category</t>
+  </si>
+  <si>
+    <t>channel1_fluorophore</t>
+  </si>
+  <si>
+    <t>channel2_fluorophore</t>
+  </si>
+  <si>
+    <t>ANKCJTF</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1633GA</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1633_A</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1633_G</t>
+  </si>
+  <si>
+    <t>variant</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>FAM</t>
+  </si>
+  <si>
+    <t>VIC</t>
+  </si>
+  <si>
+    <t>ANU7H7Y</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1033AG</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1033_G</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1033_A</t>
+  </si>
+  <si>
+    <t>ANCFJNC</t>
+  </si>
+  <si>
+    <t>SMO_c.1234CT</t>
+  </si>
+  <si>
+    <t>SMO_c.1234_T</t>
+  </si>
+  <si>
+    <t>SMO_c.1234_C</t>
+  </si>
+  <si>
+    <t>ANGZVVH</t>
+  </si>
+  <si>
+    <t>GNAQ_c.548GA</t>
+  </si>
+  <si>
+    <t>GNAQ_c.548_A</t>
+  </si>
+  <si>
+    <t>GNAQ_c.548_G</t>
+  </si>
+  <si>
+    <t>ANH6PFF</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1357GA</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1357_A</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1357_G</t>
+  </si>
+  <si>
+    <t>ANEP7PN</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1624GA</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1624_A</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1624_G</t>
+  </si>
+  <si>
+    <t>ANKCHZD</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.263GA</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.263_A</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.263_G</t>
+  </si>
+  <si>
+    <t>ANWDCMH</t>
+  </si>
+  <si>
+    <t>GNA11_c.547CT</t>
+  </si>
+  <si>
+    <t>GNA11_c.547_T</t>
+  </si>
+  <si>
+    <t>GNA11_c.547_C</t>
+  </si>
+  <si>
+    <t>ANMGCUE</t>
+  </si>
+  <si>
+    <t>GNASc601CT</t>
+  </si>
+  <si>
+    <t>GNAS_c.601_T</t>
+  </si>
+  <si>
+    <t>GNAS_c.601_C</t>
+  </si>
+  <si>
+    <t>ANNK6EC</t>
+  </si>
+  <si>
+    <t>GNASc602GA</t>
+  </si>
+  <si>
+    <t>GNAS_c.602_A</t>
+  </si>
+  <si>
+    <t>GNAS_c.602_G</t>
+  </si>
+  <si>
+    <t>ANCFJRY</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.2816AG</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.2816_G</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.2816_A</t>
+  </si>
+  <si>
+    <t>ANDKD4R</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1810TC</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1810_C</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1810_T</t>
+  </si>
+  <si>
+    <t>ANMGEDD</t>
+  </si>
+  <si>
+    <t>GNA11_c.626AT</t>
+  </si>
+  <si>
+    <t>GNA11_c.626_T</t>
+  </si>
+  <si>
+    <t>GNA11_c.626_A</t>
+  </si>
+  <si>
+    <t>AN49C9F</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1634AG</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1634_G</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1634_A</t>
+  </si>
+  <si>
+    <t>ANPR2G7</t>
+  </si>
+  <si>
+    <t>MAP2K1_c.171GT</t>
+  </si>
+  <si>
+    <t>MAP2K1_c.171_T</t>
+  </si>
+  <si>
+    <t>MAP2K1_c.171_G</t>
+  </si>
+  <si>
+    <t>ANT2PM2</t>
+  </si>
+  <si>
+    <t>MAP2K1_c.607GA</t>
+  </si>
+  <si>
+    <t>MAP2K1_c.607_A</t>
+  </si>
+  <si>
+    <t>MAP2K1_c.607_G</t>
+  </si>
+  <si>
+    <t>ANMGDKA</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1030GA</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1030_A</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1030_G</t>
+  </si>
+  <si>
+    <t>ANNK647</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.3140AG</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.3140_G</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.3140_A</t>
+  </si>
+  <si>
+    <t>ANMGFCN</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.3140AT</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.3140_T</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.3140_A2</t>
+  </si>
+  <si>
+    <t>ANFV2AK</t>
+  </si>
+  <si>
+    <t>NF1_c.1246CT</t>
+  </si>
+  <si>
+    <t>NF1_c.1246_T</t>
+  </si>
+  <si>
+    <t>NF1_c.1246_C</t>
+  </si>
+  <si>
+    <t>ANEP994</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.353GA</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.353_A</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.353_G</t>
+  </si>
+  <si>
+    <t>ANT2RFN</t>
+  </si>
+  <si>
+    <t>NF1_c7863ins</t>
+  </si>
+  <si>
+    <t>NF1_c.7863_7864ins</t>
+  </si>
+  <si>
+    <t>NF1_c.7863_7864wt</t>
+  </si>
+  <si>
+    <t>ANDKFN7</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1132TC</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1132_C</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1132_T</t>
+  </si>
+  <si>
+    <t>ANT2RMD</t>
+  </si>
+  <si>
+    <t>RHOA_c.514GA</t>
+  </si>
+  <si>
+    <t>RHOA_c.514_A</t>
+  </si>
+  <si>
+    <t>RHOA_c.514_G</t>
+  </si>
+  <si>
+    <t>ANDKF7V</t>
+  </si>
+  <si>
+    <t>ANPR3GH</t>
+  </si>
+  <si>
+    <t>ACTB_c.439CT</t>
+  </si>
+  <si>
+    <t>ACTB_c.439_T</t>
+  </si>
+  <si>
+    <t>ACTB_c.439_C</t>
+  </si>
+  <si>
+    <t>AN9H2PA</t>
+  </si>
+  <si>
+    <t>ANWDET7</t>
+  </si>
+  <si>
+    <t>ACTB_c.441insGGT</t>
+  </si>
+  <si>
+    <t>ACTB_c.441_442insGGT</t>
+  </si>
+  <si>
+    <t>ACTB_c.441_442</t>
+  </si>
+  <si>
+    <t>ANT2RMH</t>
+  </si>
+  <si>
+    <t>ANFV4DP</t>
+  </si>
+  <si>
+    <t>IDH1_c.394CT</t>
+  </si>
+  <si>
+    <t>IDH1_c.394_T</t>
+  </si>
+  <si>
+    <t>IDH1_c.394_C</t>
+  </si>
+  <si>
+    <t>ANXG9C4</t>
+  </si>
+  <si>
+    <t>HRAS_c.37GC</t>
+  </si>
+  <si>
+    <t>HRAS_c.37_C</t>
+  </si>
+  <si>
+    <t>HRAS_c.37_G</t>
+  </si>
+  <si>
+    <t>ANERATT</t>
+  </si>
+  <si>
+    <t>ANNK9WK</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1252GA</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1252_A</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1252_G</t>
+  </si>
+  <si>
+    <t>ANXG9XT</t>
+  </si>
+  <si>
+    <t>KRT10_c.467GA</t>
+  </si>
+  <si>
+    <t>KRT10_c.467_A</t>
+  </si>
+  <si>
+    <t>KRT10_c.467_G</t>
+  </si>
+  <si>
+    <t>ANXG9XZ</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.3129GA</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.3129_A</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.3129_G</t>
+  </si>
+  <si>
+    <t>AN2XRNJ</t>
+  </si>
+  <si>
+    <t>ANZTW3M</t>
+  </si>
+  <si>
+    <t>AN33J9G</t>
+  </si>
+  <si>
+    <t>ANU7KT6</t>
+  </si>
+  <si>
+    <t>KRT10_c.466CT</t>
+  </si>
+  <si>
+    <t>NRAS_c.181CA</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.2176GA</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.2740GA</t>
+  </si>
+  <si>
+    <t>KRT10_c.466_T</t>
+  </si>
+  <si>
+    <t>KRT10_c.466_C</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.2176_G</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.2740_G</t>
+  </si>
+  <si>
+    <t>NRAS_c.181_A</t>
+  </si>
+  <si>
+    <t>NRAS_c.181_C</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.2176_A</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.2740_A</t>
+  </si>
+  <si>
+    <t>BRAF_c.1799TA</t>
+  </si>
+  <si>
+    <t>ANYM3HX</t>
+  </si>
+  <si>
+    <t>ANCFJJU</t>
+  </si>
+  <si>
+    <t>KRAS_c.35GA</t>
+  </si>
+  <si>
+    <t>BRAF_c.1799_A</t>
+  </si>
+  <si>
+    <t>BRAF_c.1799_T</t>
+  </si>
+  <si>
+    <t>KRAS_c.35_A</t>
+  </si>
+  <si>
+    <t>KRAS_c.35_G</t>
+  </si>
+  <si>
     <t>channel1_target</t>
   </si>
   <si>
-    <t>channel2_target</t>
-  </si>
-  <si>
-    <t>channel1_category</t>
-  </si>
-  <si>
-    <t>channel2_category</t>
-  </si>
-  <si>
-    <t>channel1_fluorophore</t>
-  </si>
-  <si>
-    <t>channel2_fluorophore</t>
-  </si>
-  <si>
-    <t>ANKCJTF</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1633GA</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1633_A</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1633_G</t>
-  </si>
-  <si>
-    <t>variant</t>
-  </si>
-  <si>
-    <t>reference</t>
-  </si>
-  <si>
-    <t>FAM</t>
-  </si>
-  <si>
-    <t>VIC</t>
-  </si>
-  <si>
-    <t>ANU7H7Y</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1033AG</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1033_G</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1033_A</t>
-  </si>
-  <si>
-    <t>ANCFJNC</t>
-  </si>
-  <si>
-    <t>SMO_c.1234CT</t>
-  </si>
-  <si>
-    <t>SMO_c.1234_T</t>
-  </si>
-  <si>
-    <t>SMO_c.1234_C</t>
-  </si>
-  <si>
-    <t>ANGZVVH</t>
-  </si>
-  <si>
-    <t>GNAQ_c.548GA</t>
-  </si>
-  <si>
-    <t>GNAQ_c.548_A</t>
-  </si>
-  <si>
-    <t>GNAQ_c.548_G</t>
-  </si>
-  <si>
-    <t>ANH6PFF</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1357GA</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1357_A</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1357_G</t>
-  </si>
-  <si>
-    <t>ANEP7PN</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1624GA</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1624_A</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1624_G</t>
-  </si>
-  <si>
-    <t>ANKCHZD</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.263GA</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.263_A</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.263_G</t>
-  </si>
-  <si>
-    <t>ANWDCMH</t>
-  </si>
-  <si>
-    <t>GNA11_c.547CT</t>
-  </si>
-  <si>
-    <t>GNA11_c.547_T</t>
-  </si>
-  <si>
-    <t>GNA11_c.547_C</t>
-  </si>
-  <si>
-    <t>ANMGCUE</t>
-  </si>
-  <si>
-    <t>GNASc601CT</t>
-  </si>
-  <si>
-    <t>GNAS_c.601_T</t>
-  </si>
-  <si>
-    <t>GNAS_c.601_C</t>
-  </si>
-  <si>
-    <t>ANNK6EC</t>
-  </si>
-  <si>
-    <t>GNASc602GA</t>
-  </si>
-  <si>
-    <t>GNAS_c.602_A</t>
-  </si>
-  <si>
-    <t>GNAS_c.602_G</t>
-  </si>
-  <si>
-    <t>ANCFJRY</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.2816AG</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.2816_G</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.2816_A</t>
-  </si>
-  <si>
-    <t>ANDKD4R</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1810TC</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1810_C</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1810_T</t>
-  </si>
-  <si>
-    <t>ANMGEDD</t>
-  </si>
-  <si>
-    <t>GNA11_c.626AT</t>
-  </si>
-  <si>
-    <t>GNA11_c.626_T</t>
-  </si>
-  <si>
-    <t>GNA11_c.626_A</t>
-  </si>
-  <si>
-    <t>AN49C9F</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1634AG</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1634_G</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1634_A</t>
-  </si>
-  <si>
-    <t>ANPR2G7</t>
-  </si>
-  <si>
-    <t>MAP2K1_c.171GT</t>
-  </si>
-  <si>
-    <t>MAP2K1_c.171_T</t>
-  </si>
-  <si>
-    <t>MAP2K1_c.171_G</t>
-  </si>
-  <si>
-    <t>ANT2PM2</t>
-  </si>
-  <si>
-    <t>MAP2K1_c.607GA</t>
-  </si>
-  <si>
-    <t>MAP2K1_c.607_A</t>
-  </si>
-  <si>
-    <t>MAP2K1_c.607_G</t>
-  </si>
-  <si>
-    <t>ANMGDKA</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1030GA</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1030_A</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1030_G</t>
-  </si>
-  <si>
-    <t>ANNK647</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.3140AG</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.3140_G</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.3140_A</t>
-  </si>
-  <si>
-    <t>ANMGFCN</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.3140AT</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.3140_T</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.3140_A2</t>
-  </si>
-  <si>
-    <t>ANFV2AK</t>
-  </si>
-  <si>
-    <t>NF1_c.1246CT</t>
-  </si>
-  <si>
-    <t>NF1_c.1246_T</t>
-  </si>
-  <si>
-    <t>NF1_c.1246_C</t>
-  </si>
-  <si>
-    <t>ANEP994</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.353GA</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.353_A</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.353_G</t>
-  </si>
-  <si>
-    <t>ANT2RFN</t>
-  </si>
-  <si>
-    <t>NF1_c7863ins</t>
-  </si>
-  <si>
-    <t>NF1_c.7863_7864ins</t>
-  </si>
-  <si>
-    <t>NF1_c.7863_7864wt</t>
-  </si>
-  <si>
-    <t>ANDKFN7</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1132TC</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1132_C</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1132_T</t>
-  </si>
-  <si>
-    <t>ANT2RMD</t>
-  </si>
-  <si>
-    <t>RHOA_c.514GA</t>
-  </si>
-  <si>
-    <t>RHOA_c.514_A</t>
-  </si>
-  <si>
-    <t>RHOA_c.514_G</t>
-  </si>
-  <si>
-    <t>ANDKF7V</t>
-  </si>
-  <si>
-    <t>ANPR3GH</t>
-  </si>
-  <si>
-    <t>ACTB_c.439CT</t>
-  </si>
-  <si>
-    <t>ACTB_c.439_T</t>
-  </si>
-  <si>
-    <t>ACTB_c.439_C</t>
-  </si>
-  <si>
-    <t>AN9H2PA</t>
-  </si>
-  <si>
-    <t>ANWDET7</t>
-  </si>
-  <si>
-    <t>ACTB_c.441insGGT</t>
-  </si>
-  <si>
-    <t>ACTB_c.441_442insGGT</t>
-  </si>
-  <si>
-    <t>ACTB_c.441_442</t>
-  </si>
-  <si>
-    <t>ANT2RMH</t>
-  </si>
-  <si>
-    <t>ANFV4DP</t>
-  </si>
-  <si>
-    <t>IDH1_c.394CT</t>
-  </si>
-  <si>
-    <t>IDH1_c.394_T</t>
-  </si>
-  <si>
-    <t>IDH1_c.394_C</t>
-  </si>
-  <si>
-    <t>ANXG9C4</t>
-  </si>
-  <si>
-    <t>HRAS_c.37GC</t>
-  </si>
-  <si>
-    <t>HRAS_c.37_C</t>
-  </si>
-  <si>
-    <t>HRAS_c.37_G</t>
-  </si>
-  <si>
-    <t>ANERATT</t>
-  </si>
-  <si>
-    <t>ANNK9WK</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1252GA</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1252_A</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.1252_G</t>
-  </si>
-  <si>
-    <t>ANXG9XT</t>
-  </si>
-  <si>
-    <t>KRT10_c.467GA</t>
-  </si>
-  <si>
-    <t>KRT10_c.467_A</t>
-  </si>
-  <si>
-    <t>KRT10_c.467_G</t>
-  </si>
-  <si>
-    <t>ANXG9XZ</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.3129GA</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.3129_A</t>
-  </si>
-  <si>
-    <t>PIK3CA_c.3129_G</t>
+    <t>ANWDFD3</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1133GA</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1133_A</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1133_G</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1092,18 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1335,10 +1430,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,937 +1455,1122 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>46</v>
       </c>
-      <c r="D10" t="s">
-        <v>47</v>
-      </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
         <v>52</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>53</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>54</v>
       </c>
-      <c r="D12" t="s">
-        <v>55</v>
-      </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
         <v>56</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>57</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>58</v>
       </c>
-      <c r="D13" t="s">
-        <v>59</v>
-      </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
         <v>60</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>61</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>62</v>
       </c>
-      <c r="D14" t="s">
-        <v>63</v>
-      </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>65</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>66</v>
       </c>
-      <c r="D15" t="s">
-        <v>67</v>
-      </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
         <v>68</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>69</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>70</v>
       </c>
-      <c r="D16" t="s">
-        <v>71</v>
-      </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
         <v>72</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>73</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>74</v>
       </c>
-      <c r="D17" t="s">
-        <v>75</v>
-      </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s">
         <v>76</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>77</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>78</v>
       </c>
-      <c r="D18" t="s">
-        <v>79</v>
-      </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" t="s">
         <v>80</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>81</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>82</v>
       </c>
-      <c r="D19" t="s">
-        <v>83</v>
-      </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" t="s">
         <v>84</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>85</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>86</v>
       </c>
-      <c r="D20" t="s">
-        <v>87</v>
-      </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
         <v>88</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>89</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>90</v>
       </c>
-      <c r="D21" t="s">
-        <v>91</v>
-      </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
         <v>92</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>93</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>94</v>
       </c>
-      <c r="D22" t="s">
-        <v>95</v>
-      </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" t="s">
         <v>96</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>97</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>98</v>
       </c>
-      <c r="D23" t="s">
-        <v>99</v>
-      </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" t="s">
         <v>100</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>101</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>102</v>
       </c>
-      <c r="D24" t="s">
-        <v>103</v>
-      </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" t="s">
         <v>104</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>105</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>106</v>
       </c>
-      <c r="D25" t="s">
-        <v>107</v>
-      </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" t="s">
         <v>105</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>106</v>
       </c>
-      <c r="D26" t="s">
-        <v>107</v>
-      </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" t="s">
         <v>109</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>110</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>111</v>
       </c>
-      <c r="D27" t="s">
-        <v>112</v>
-      </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" t="s">
         <v>110</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>111</v>
       </c>
-      <c r="D28" t="s">
-        <v>112</v>
-      </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" t="s">
         <v>114</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>115</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>116</v>
       </c>
-      <c r="D29" t="s">
-        <v>117</v>
-      </c>
       <c r="E29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" t="s">
         <v>115</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>116</v>
       </c>
-      <c r="D30" t="s">
-        <v>117</v>
-      </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" t="s">
         <v>119</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>120</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>121</v>
       </c>
-      <c r="D31" t="s">
-        <v>122</v>
-      </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" t="s">
         <v>123</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>124</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>125</v>
       </c>
-      <c r="D32" t="s">
-        <v>126</v>
-      </c>
       <c r="E32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" t="s">
         <v>124</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>125</v>
       </c>
-      <c r="D33" t="s">
-        <v>126</v>
-      </c>
       <c r="E33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" t="s">
         <v>128</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>129</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>130</v>
       </c>
-      <c r="D34" t="s">
-        <v>131</v>
-      </c>
       <c r="E34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" t="s">
         <v>132</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>133</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>134</v>
       </c>
-      <c r="D35" t="s">
-        <v>135</v>
-      </c>
       <c r="E35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" t="s">
         <v>136</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>137</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>138</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" t="s">
+        <v>148</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>141</v>
+      </c>
+      <c r="B38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D38" t="s">
+        <v>152</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39" t="s">
+        <v>153</v>
+      </c>
+      <c r="D39" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>139</v>
       </c>
-      <c r="E36" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" t="s">
-        <v>15</v>
+      <c r="B40" t="s">
+        <v>146</v>
+      </c>
+      <c r="C40" t="s">
+        <v>154</v>
+      </c>
+      <c r="D40" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" t="s">
+        <v>159</v>
+      </c>
+      <c r="D41" t="s">
+        <v>160</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>157</v>
+      </c>
+      <c r="B42" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" t="s">
+        <v>161</v>
+      </c>
+      <c r="D42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>164</v>
+      </c>
+      <c r="B43" t="s">
+        <v>165</v>
+      </c>
+      <c r="C43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576 E2:E1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"variant,reference"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">

</xml_diff>

<commit_message>
Addition of patient demographics and update with 2 most recent ddPCR runs.
</commit_message>
<xml_diff>
--- a/resources/mosaic_targets_v2.xlsx
+++ b/resources/mosaic_targets_v2.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Regional Genetics Service\Validation Documents\Mosaic\ddPCR\ddpcr_mosaicism\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D1451C-C5BE-4AA9-A56B-C34C31E4AA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBBDDCD-5111-4E1C-B60E-864122B0B2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mosaicism_targets_v2" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">mosaicism_targets_v2!$A$1:$H$48</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -58,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="221">
   <si>
     <t>assay_id</t>
   </si>
@@ -562,6 +565,165 @@
   </si>
   <si>
     <t>PIK3CA_c.1133_G</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.2953TA</t>
+  </si>
+  <si>
+    <t>KRAS_c.436GA</t>
+  </si>
+  <si>
+    <t>MAP2K1_c.168GT</t>
+  </si>
+  <si>
+    <t>RASA1_c1493_9del</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.2953A</t>
+  </si>
+  <si>
+    <t>KRAS_c.436A</t>
+  </si>
+  <si>
+    <t>MAP2K1_c.168T</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.2953T</t>
+  </si>
+  <si>
+    <t>KRAS_c.436G</t>
+  </si>
+  <si>
+    <t>MAP2K1_c.168G</t>
+  </si>
+  <si>
+    <t>RASA1_c1493_9</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1034T</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1034A</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1034AT</t>
+  </si>
+  <si>
+    <t>ANPR4AR</t>
+  </si>
+  <si>
+    <t>ANZTXEG</t>
+  </si>
+  <si>
+    <t>AN2XRYE</t>
+  </si>
+  <si>
+    <t>NF1_c.4330AG</t>
+  </si>
+  <si>
+    <t>AN33KJC</t>
+  </si>
+  <si>
+    <t>MTOR_c.4376CA</t>
+  </si>
+  <si>
+    <t>AN49E39</t>
+  </si>
+  <si>
+    <t>RASA1_c.1192CT</t>
+  </si>
+  <si>
+    <t>AN7D9N6</t>
+  </si>
+  <si>
+    <t>GNAQ_c.547CG</t>
+  </si>
+  <si>
+    <t>AN9H293</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1258TC</t>
+  </si>
+  <si>
+    <t>ANH6T4N</t>
+  </si>
+  <si>
+    <t>NRAS_c.182AG</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1034_T</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1034_A</t>
+  </si>
+  <si>
+    <t>NF1_c.4330_A</t>
+  </si>
+  <si>
+    <t>MTOR_c.4376_A</t>
+  </si>
+  <si>
+    <t>NRAS_c.182_A</t>
+  </si>
+  <si>
+    <t>NF1_c.4330_G</t>
+  </si>
+  <si>
+    <t>MTOR_c.4376_C</t>
+  </si>
+  <si>
+    <t>RASA1_c.1192_T</t>
+  </si>
+  <si>
+    <t>RASA1_c.1192_C</t>
+  </si>
+  <si>
+    <t>GNAQ_c.547_C</t>
+  </si>
+  <si>
+    <t>GNAQ_c.547_G</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1258_C</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1258_T</t>
+  </si>
+  <si>
+    <t>NRAS_c.182_G</t>
+  </si>
+  <si>
+    <t>AN7D6UD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	PIK3CA_c.2908GA</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.2908_A</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.2908_G</t>
+  </si>
+  <si>
+    <t>ANMGF4W</t>
+  </si>
+  <si>
+    <t>ANNMAPU</t>
+  </si>
+  <si>
+    <t>ANRWXVN</t>
+  </si>
+  <si>
+    <t>ANKCMJY</t>
+  </si>
+  <si>
+    <t>NF1_c.7863_7864</t>
+  </si>
+  <si>
+    <t>ACTB_c.1043_1044ins18</t>
+  </si>
+  <si>
+    <t>ACTB_c.1043_1044</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1254,267 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1430,16 +1852,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
@@ -2565,22 +2987,484 @@
         <v>14</v>
       </c>
     </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>214</v>
+      </c>
+      <c r="B44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C44" t="s">
+        <v>172</v>
+      </c>
+      <c r="D44" t="s">
+        <v>175</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>215</v>
+      </c>
+      <c r="B45" t="s">
+        <v>169</v>
+      </c>
+      <c r="C45" t="s">
+        <v>173</v>
+      </c>
+      <c r="D45" t="s">
+        <v>176</v>
+      </c>
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>216</v>
+      </c>
+      <c r="B46" t="s">
+        <v>170</v>
+      </c>
+      <c r="C46" t="s">
+        <v>174</v>
+      </c>
+      <c r="D46" t="s">
+        <v>177</v>
+      </c>
+      <c r="E46" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>217</v>
+      </c>
+      <c r="B47" t="s">
+        <v>171</v>
+      </c>
+      <c r="C47" t="s">
+        <v>171</v>
+      </c>
+      <c r="D47" t="s">
+        <v>178</v>
+      </c>
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>182</v>
+      </c>
+      <c r="B48" t="s">
+        <v>181</v>
+      </c>
+      <c r="C48" t="s">
+        <v>179</v>
+      </c>
+      <c r="D48" t="s">
+        <v>180</v>
+      </c>
+      <c r="E48" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>183</v>
+      </c>
+      <c r="B49" t="s">
+        <v>181</v>
+      </c>
+      <c r="C49" t="s">
+        <v>196</v>
+      </c>
+      <c r="D49" t="s">
+        <v>197</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>184</v>
+      </c>
+      <c r="B50" t="s">
+        <v>185</v>
+      </c>
+      <c r="C50" t="s">
+        <v>201</v>
+      </c>
+      <c r="D50" t="s">
+        <v>198</v>
+      </c>
+      <c r="E50" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>186</v>
+      </c>
+      <c r="B51" t="s">
+        <v>187</v>
+      </c>
+      <c r="C51" t="s">
+        <v>199</v>
+      </c>
+      <c r="D51" t="s">
+        <v>202</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>188</v>
+      </c>
+      <c r="B52" t="s">
+        <v>189</v>
+      </c>
+      <c r="C52" t="s">
+        <v>203</v>
+      </c>
+      <c r="D52" t="s">
+        <v>204</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" t="s">
+        <v>13</v>
+      </c>
+      <c r="H52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53" t="s">
+        <v>191</v>
+      </c>
+      <c r="C53" t="s">
+        <v>206</v>
+      </c>
+      <c r="D53" t="s">
+        <v>205</v>
+      </c>
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" t="s">
+        <v>13</v>
+      </c>
+      <c r="H53" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>192</v>
+      </c>
+      <c r="B54" t="s">
+        <v>193</v>
+      </c>
+      <c r="C54" t="s">
+        <v>207</v>
+      </c>
+      <c r="D54" t="s">
+        <v>208</v>
+      </c>
+      <c r="E54" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" t="s">
+        <v>13</v>
+      </c>
+      <c r="H54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>194</v>
+      </c>
+      <c r="B55" t="s">
+        <v>195</v>
+      </c>
+      <c r="C55" t="s">
+        <v>209</v>
+      </c>
+      <c r="D55" t="s">
+        <v>200</v>
+      </c>
+      <c r="E55" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" t="s">
+        <v>12</v>
+      </c>
+      <c r="G55" t="s">
+        <v>13</v>
+      </c>
+      <c r="H55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>210</v>
+      </c>
+      <c r="B56" t="s">
+        <v>211</v>
+      </c>
+      <c r="C56" t="s">
+        <v>212</v>
+      </c>
+      <c r="D56" t="s">
+        <v>213</v>
+      </c>
+      <c r="E56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" t="s">
+        <v>13</v>
+      </c>
+      <c r="H56" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" t="s">
+        <v>218</v>
+      </c>
+      <c r="D57" t="s">
+        <v>97</v>
+      </c>
+      <c r="E57" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>219</v>
+      </c>
+      <c r="B58" t="s">
+        <v>219</v>
+      </c>
+      <c r="C58" t="s">
+        <v>220</v>
+      </c>
+      <c r="D58" t="s">
+        <v>219</v>
+      </c>
+      <c r="E58" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" t="s">
+        <v>13</v>
+      </c>
+      <c r="H58" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <autoFilter ref="A1:H48" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="A50:A56 A1:A48 A59:A1048576">
+    <cfRule type="duplicateValues" dxfId="26" priority="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:B56 A62:B1048576 A60:A61 A48 A1:B47 A59:B59">
+    <cfRule type="duplicateValues" dxfId="25" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A56 A59:A1048576">
+    <cfRule type="duplicateValues" dxfId="24" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="29"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44:D47">
+    <cfRule type="duplicateValues" dxfId="22" priority="55"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A56 A59:A1048576">
+    <cfRule type="duplicateValues" dxfId="21" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50">
+    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D52">
+    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55">
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55">
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57:A58">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57:A58">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57:A58">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57:A58">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"variant,reference"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"FAM"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"VIC,HEX"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C60:C61 E62:F1048576 F60:F61 E2:F59 C57:C58" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"variant,reference"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update to targets file
</commit_message>
<xml_diff>
--- a/resources/mosaic_targets_v2.xlsx
+++ b/resources/mosaic_targets_v2.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Regional Genetics Service\Validation Documents\Mosaic\ddPCR\ddpcr_mosaicism\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBBDDCD-5111-4E1C-B60E-864122B0B2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33F3451-24D0-47FE-905D-5CAE6892923E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mosaicism_targets_v2" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">mosaicism_targets_v2!$A$1:$H$48</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="237">
   <si>
     <t>assay_id</t>
   </si>
@@ -724,6 +725,54 @@
   </si>
   <si>
     <t>ACTB_c.1043_1044</t>
+  </si>
+  <si>
+    <t>ANU7K7Y</t>
+  </si>
+  <si>
+    <t>NF1_c.1885GA</t>
+  </si>
+  <si>
+    <t>ANWDFTW</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1035TA</t>
+  </si>
+  <si>
+    <t>ANXHADU</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.323GA</t>
+  </si>
+  <si>
+    <t>ANYM3XR</t>
+  </si>
+  <si>
+    <t>NRAS_c.34GC</t>
+  </si>
+  <si>
+    <t>NF1_c.1885_A</t>
+  </si>
+  <si>
+    <t>NF1_c.1885_G</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1035_T</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.323_G</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.1035_A</t>
+  </si>
+  <si>
+    <t>PIK3CA_c.323_A</t>
+  </si>
+  <si>
+    <t>NRAS_c.34_C</t>
+  </si>
+  <si>
+    <t>NRAS_c.34_G</t>
   </si>
 </sst>
 </file>
@@ -1254,7 +1303,27 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1852,11 +1921,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3377,94 +3446,225 @@
         <v>14</v>
       </c>
     </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>221</v>
+      </c>
+      <c r="B59" t="s">
+        <v>222</v>
+      </c>
+      <c r="C59" t="s">
+        <v>229</v>
+      </c>
+      <c r="D59" t="s">
+        <v>230</v>
+      </c>
+      <c r="E59" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>223</v>
+      </c>
+      <c r="B60" t="s">
+        <v>224</v>
+      </c>
+      <c r="C60" t="s">
+        <v>233</v>
+      </c>
+      <c r="D60" t="s">
+        <v>231</v>
+      </c>
+      <c r="E60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>225</v>
+      </c>
+      <c r="B61" t="s">
+        <v>226</v>
+      </c>
+      <c r="C61" t="s">
+        <v>234</v>
+      </c>
+      <c r="D61" t="s">
+        <v>232</v>
+      </c>
+      <c r="E61" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" t="s">
+        <v>12</v>
+      </c>
+      <c r="G61" t="s">
+        <v>13</v>
+      </c>
+      <c r="H61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>227</v>
+      </c>
+      <c r="B62" t="s">
+        <v>228</v>
+      </c>
+      <c r="C62" t="s">
+        <v>235</v>
+      </c>
+      <c r="D62" t="s">
+        <v>236</v>
+      </c>
+      <c r="E62" t="s">
+        <v>11</v>
+      </c>
+      <c r="F62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H62" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H48" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A50:A56 A1:A48 A59:A1048576">
-    <cfRule type="duplicateValues" dxfId="26" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:B56 A62:B1048576 A60:A61 A48 A1:B47 A59:B59">
-    <cfRule type="duplicateValues" dxfId="25" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A56 A59:A1048576">
-    <cfRule type="duplicateValues" dxfId="24" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44:D47">
-    <cfRule type="duplicateValues" dxfId="22" priority="55"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A56 A59:A1048576">
-    <cfRule type="duplicateValues" dxfId="21" priority="22"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
+    <cfRule type="duplicateValues" dxfId="23" priority="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50">
+    <cfRule type="duplicateValues" dxfId="22" priority="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="duplicateValues" dxfId="21" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="duplicateValues" dxfId="20" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
     <cfRule type="duplicateValues" dxfId="19" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D50">
+  <conditionalFormatting sqref="D52">
     <cfRule type="duplicateValues" dxfId="18" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
+  <conditionalFormatting sqref="C53">
     <cfRule type="duplicateValues" dxfId="17" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
+  <conditionalFormatting sqref="D53">
     <cfRule type="duplicateValues" dxfId="16" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
+  <conditionalFormatting sqref="C54">
     <cfRule type="duplicateValues" dxfId="15" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
+  <conditionalFormatting sqref="D54">
     <cfRule type="duplicateValues" dxfId="14" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
+  <conditionalFormatting sqref="C55">
     <cfRule type="duplicateValues" dxfId="13" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
+  <conditionalFormatting sqref="D55">
     <cfRule type="duplicateValues" dxfId="12" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
+  <conditionalFormatting sqref="C56">
     <cfRule type="duplicateValues" dxfId="11" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
+  <conditionalFormatting sqref="D56">
     <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
+  <conditionalFormatting sqref="A57:A58">
     <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
+  <conditionalFormatting sqref="A57:A58">
     <cfRule type="duplicateValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  <conditionalFormatting sqref="A57:A58">
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:A58">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A57:A58">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A57:A58">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  <conditionalFormatting sqref="D59">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A57:A58">
+  <conditionalFormatting sqref="C62">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C57:C58 E2:F1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"variant,reference"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"FAM"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"VIC,HEX"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C60:C61 E62:F1048576 F60:F61 E2:F59 C57:C58" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"variant,reference"</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88394D09-CEDD-4AAE-8B60-7D6EAAEB8BE2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>